<commit_message>
Typo fix, TestManager filled
</commit_message>
<xml_diff>
--- a/TestManager.xlsx
+++ b/TestManager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Automation Curse\Week 4\remek_alm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3342FAD9-037E-4DC5-A1DB-5DBA36D6D1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A817796-5AC6-483A-A8FE-2559C882DFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
   <si>
     <t>Azonosító (ID)</t>
   </si>
@@ -114,49 +114,19 @@
     <t>Almáshegyi Leó</t>
   </si>
   <si>
-    <t>1. Leave field 'a' empty
-2. Type in field 'b'
-3. Click 'Get Total'</t>
-  </si>
-  <si>
     <t>TC2</t>
-  </si>
-  <si>
-    <t>1. Leave field 'b' empty
-2. Type in field 'a'
-3. Click 'Get Total'</t>
   </si>
   <si>
     <t>TC3</t>
   </si>
   <si>
-    <t>1. Type integer into field 'a'
-2. Type integer into field 'b'
-3. Click 'Get Total'</t>
-  </si>
-  <si>
     <t>TC4</t>
-  </si>
-  <si>
-    <t>1. Type float into field 'a'
-2. Type float into field 'b'
-3. Click 'Get Total'</t>
   </si>
   <si>
     <t>TC5</t>
   </si>
   <si>
-    <t>1. Type in field 'a'
-2. Type in field 'b'
-3. Click 'Get Total'</t>
-  </si>
-  <si>
     <t>TC6</t>
-  </si>
-  <si>
-    <t>1. Leave field 'a' empty
-2. Leave field 'b' empty
-3. Click 'Get Total'</t>
   </si>
   <si>
     <t>TC7</t>
@@ -165,17 +135,7 @@
     <t>TC8</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Type integer into field 'a'
-2. Type integer into field 'b'
-3. Press 'Enter' </t>
-  </si>
-  <si>
     <t>TC9</t>
-  </si>
-  <si>
-    <t>1. Type a simple operation inside field 'a'
-2. Type a simple operation inside field 'b'
-3. Click 'Get Total'</t>
   </si>
   <si>
     <t>TC10</t>
@@ -236,6 +196,158 @@
   </si>
   <si>
     <t>URL - https://lennertamas.github.io/portio/</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Registration of new user</t>
+  </si>
+  <si>
+    <t>username = kosza
+password = lajos
+email = kosza.lajos@citromail.hu
+description = Just your average Lajos</t>
+  </si>
+  <si>
+    <t>1. Navigate to page
+2. Accept 'Terms and Conditions'
+3. Select 'Register' tab
+4. Fill in required fields
+5. Click 'Register' button</t>
+  </si>
+  <si>
+    <t>Successful registration' message appears</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Login with newly created user</t>
+  </si>
+  <si>
+    <t>1. Register a new user as in TC1
+2. Navigate to 'Login' tab
+3. Fill in required fields
+4. Click 'Login' button</t>
+  </si>
+  <si>
+    <t>User logs into the site, 'Log out' button is visible</t>
+  </si>
+  <si>
+    <t>Magas</t>
+  </si>
+  <si>
+    <t>Login with existing user</t>
+  </si>
+  <si>
+    <t>1. Navigate to page
+2. Accept 'Terms and Conditions'
+3. Fill in required fields
+4. Click 'Login' button</t>
+  </si>
+  <si>
+    <t>username = lovasia
+password = kispal123</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Logout from account</t>
+  </si>
+  <si>
+    <t>1. Register and login with new user as in TC2
+2. Click 'Logout' button</t>
+  </si>
+  <si>
+    <t>User successfully logs out, log in page is visible</t>
+  </si>
+  <si>
+    <t>Alacsony</t>
+  </si>
+  <si>
+    <t>Edit profile</t>
+  </si>
+  <si>
+    <t>Editing profile information</t>
+  </si>
+  <si>
+    <t>1. Register and login with new user as in TC2
+2. Click 'Edit Profile' button
+3. Fill in required fields
+4. Click 'Save' button</t>
+  </si>
+  <si>
+    <t>name = jozsi
+bio = Below average student
+phone = 11111111111</t>
+  </si>
+  <si>
+    <t>Confirmation message appears about the changes</t>
+  </si>
+  <si>
+    <t>Delete profile</t>
+  </si>
+  <si>
+    <t>Deleting newly created profile</t>
+  </si>
+  <si>
+    <t>1. Register and login with new user as in TC2
+2. Click 'Edit Profile' button
+3. Click 'Delete' button
+4. Click 'Confirm Delete' button</t>
+  </si>
+  <si>
+    <t>User will be redirected to the log in page, can't log in with the previously deleted credentials</t>
+  </si>
+  <si>
+    <t>Article names</t>
+  </si>
+  <si>
+    <t>Walk through of multi-page blog, comparing article names from file</t>
+  </si>
+  <si>
+    <t>1. Login with existing user
+2. Navigate to 'Blog' tab
+3. Click 'See all post' button
+4. Get all article titles</t>
+  </si>
+  <si>
+    <t>All articles are available and their names match the content of the file found in the repository</t>
+  </si>
+  <si>
+    <t>Save image</t>
+  </si>
+  <si>
+    <t>Saving an image</t>
+  </si>
+  <si>
+    <t>1. Login with existing user
+2. Save image
+3. Delete downloaded image</t>
+  </si>
+  <si>
+    <t>User can download images from the site</t>
+  </si>
+  <si>
+    <t>Login with multiple users repeatedly from file</t>
+  </si>
+  <si>
+    <t>1. Navigate to page
+2. Accept 'Terms and Conditions'
+3. Login with multiple users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    login= lovasia
+    password= kispal123,
+    login= kisst
+    password= quimby123,
+    login= beckz
+    password= 30y123</t>
+  </si>
+  <si>
+    <t>User can log in with every user</t>
   </si>
 </sst>
 </file>
@@ -326,7 +438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -350,84 +462,15 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE598"/>
-          <bgColor rgb="FFFFE598"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE598"/>
-          <bgColor rgb="FFFFE598"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE598"/>
-          <bgColor rgb="FFFFE598"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -714,8 +757,8 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -838,22 +881,30 @@
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="D3" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="5"/>
+      <c r="H3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="J3" s="5"/>
       <c r="K3" s="6"/>
       <c r="L3" s="5"/>
@@ -873,24 +924,32 @@
     </row>
     <row r="4" spans="1:25" ht="85.5" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="D4" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="5"/>
+      <c r="H4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="J4" s="5"/>
       <c r="K4" s="6"/>
       <c r="L4" s="5"/>
@@ -910,24 +969,32 @@
     </row>
     <row r="5" spans="1:25" ht="60" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="D5" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="5"/>
+      <c r="H5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="J5" s="5"/>
       <c r="K5" s="6"/>
       <c r="L5" s="5"/>
@@ -947,12 +1014,16 @@
     </row>
     <row r="6" spans="1:25" ht="60" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="D6" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>16</v>
@@ -961,10 +1032,12 @@
         <v>24</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="H6" s="6"/>
-      <c r="I6" s="5"/>
+      <c r="I6" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="J6" s="5"/>
       <c r="K6" s="6"/>
       <c r="L6" s="5"/>
@@ -984,24 +1057,32 @@
     </row>
     <row r="7" spans="1:25" ht="60" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="D7" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="5"/>
+      <c r="H7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="J7" s="5"/>
       <c r="K7" s="6"/>
       <c r="L7" s="5"/>
@@ -1021,12 +1102,16 @@
     </row>
     <row r="8" spans="1:25" ht="60" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="D8" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>16</v>
@@ -1035,10 +1120,12 @@
         <v>24</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="H8" s="6"/>
-      <c r="I8" s="5"/>
+      <c r="I8" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="J8" s="5"/>
       <c r="K8" s="6"/>
       <c r="L8" s="5"/>
@@ -1058,24 +1145,30 @@
     </row>
     <row r="9" spans="1:25" ht="60" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="D9" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="H9" s="6"/>
-      <c r="I9" s="5"/>
+      <c r="I9" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="J9" s="5"/>
       <c r="K9" s="6"/>
       <c r="L9" s="5"/>
@@ -1095,24 +1188,30 @@
     </row>
     <row r="10" spans="1:25" ht="60" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="D10" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="H10" s="6"/>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="J10" s="5"/>
       <c r="K10" s="6"/>
       <c r="L10" s="5"/>
@@ -1132,12 +1231,16 @@
     </row>
     <row r="11" spans="1:25" ht="60" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="D11" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>16</v>
@@ -1146,10 +1249,14 @@
         <v>24</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="5"/>
+      <c r="H11" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="J11" s="5"/>
       <c r="K11" s="6"/>
       <c r="L11" s="5"/>
@@ -1169,12 +1276,12 @@
     </row>
     <row r="12" spans="1:25" ht="60" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>16</v>
@@ -7600,32 +7707,24 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="E2:E22">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E22">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E22">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K22">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K22">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K22">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7639,9 +7738,9 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D4:D9" r:id="rId2" display="URL - https://lennertamas.github.io/portio/" xr:uid="{A37D4AFC-EE51-4EB5-9205-AFDFEA61D8D8}"/>
-    <hyperlink ref="D10" r:id="rId3" xr:uid="{E270FD4A-0487-426B-BB7D-1905CC3CA50A}"/>
-    <hyperlink ref="D11:D12" r:id="rId4" display="URL - https://lennertamas.github.io/portio/" xr:uid="{FE55F378-CD03-4626-847A-11A0F9BE58A8}"/>
+    <hyperlink ref="D10" r:id="rId2" xr:uid="{E270FD4A-0487-426B-BB7D-1905CC3CA50A}"/>
+    <hyperlink ref="D11:D12" r:id="rId3" display="URL - https://lennertamas.github.io/portio/" xr:uid="{FE55F378-CD03-4626-847A-11A0F9BE58A8}"/>
+    <hyperlink ref="D4:D9" r:id="rId4" display="URL - https://lennertamas.github.io/portio/" xr:uid="{A37D4AFC-EE51-4EB5-9205-AFDFEA61D8D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -7669,16 +7768,16 @@
     <row r="1" spans="1:5" ht="15.75">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75">
@@ -7692,7 +7791,7 @@
     </row>
     <row r="3" spans="1:5" ht="45.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -7710,24 +7809,24 @@
     </row>
     <row r="5" spans="1:5" ht="48" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="48" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -7736,7 +7835,7 @@
     </row>
     <row r="7" spans="1:5" ht="48" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -7745,7 +7844,7 @@
     </row>
     <row r="8" spans="1:5" ht="48" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -7754,7 +7853,7 @@
     </row>
     <row r="9" spans="1:5" ht="48" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -7763,7 +7862,7 @@
     </row>
     <row r="10" spans="1:5" ht="48" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -7772,36 +7871,36 @@
     </row>
     <row r="11" spans="1:5" ht="48" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="48" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="48" customHeight="1">
@@ -7824,7 +7923,7 @@
     </row>
     <row r="15" spans="1:5" ht="115.5" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -13742,63 +13841,14 @@
       <c r="E1000" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+  <conditionalFormatting sqref="B6:E7">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6:E6">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6:E6">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6:E6">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7:E7">
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7:E7">
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7:E7">
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>